<commit_message>
Added code for suite sheet to execute specific tests.
</commit_message>
<xml_diff>
--- a/src/main/java/keywordDrivenFramework/priceWatchKeyword.xlsx
+++ b/src/main/java/keywordDrivenFramework/priceWatchKeyword.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chandrashekarn\TechnicalStuff\Selenium\KeywordDriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chandrashekarn\IdeaProjects\PriceWatch\src\main\java\keywordDrivenFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="suite" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t>test step</t>
   </si>
@@ -71,43 +72,115 @@
     <t>cssSelector</t>
   </si>
   <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>sendkeys</t>
+  </si>
+  <si>
+    <t>verify page url</t>
+  </si>
+  <si>
+    <t>input[name = 'Password']</t>
+  </si>
+  <si>
+    <t>.btn.btn-default</t>
+  </si>
+  <si>
+    <t>get page url</t>
+  </si>
+  <si>
+    <t>kiddyt</t>
+  </si>
+  <si>
+    <t>/trackproduct</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>a[title = 'Login to PriceWatch']</t>
   </si>
   <si>
     <t>input[name = 'UserName']</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>sendkeys</t>
-  </si>
-  <si>
-    <t>verify page url</t>
-  </si>
-  <si>
-    <t>input[name = 'Password']</t>
-  </si>
-  <si>
-    <t>.btn.btn-default</t>
-  </si>
-  <si>
-    <t>get page url</t>
-  </si>
-  <si>
-    <t>kiddyt</t>
-  </si>
-  <si>
-    <t>/trackproduct</t>
-  </si>
-  <si>
-    <t>close browser</t>
-  </si>
-  <si>
-    <t>quit</t>
-  </si>
-  <si>
-    <t>Chrome</t>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>enter invalid username</t>
+  </si>
+  <si>
+    <t>kiddytabc</t>
+  </si>
+  <si>
+    <t>123456abc</t>
+  </si>
+  <si>
+    <t>enter invalid password</t>
+  </si>
+  <si>
+    <t>verify login failure message</t>
+  </si>
+  <si>
+    <t>ERROR! - Invalid username/password.</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>saveMessage</t>
+  </si>
+  <si>
+    <t>get text</t>
+  </si>
+  <si>
+    <t>Wait for the page content</t>
+  </si>
+  <si>
+    <t>wait for page content</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>Wait for some time</t>
+  </si>
+  <si>
+    <t>sleep</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Login with valid credentails</t>
+  </si>
+  <si>
+    <t>Login with invalid credentails</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>tc_no</t>
+  </si>
+  <si>
+    <t>tc_name</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -166,10 +239,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,7 +526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -459,171 +534,454 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="51" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F19" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>